<commit_message>
Modified json files structure to make them compatible with huiji's json data schema.
</commit_message>
<xml_diff>
--- a/EnemyPartDrop.xlsx
+++ b/EnemyPartDrop.xlsx
@@ -140,6 +140,12 @@
     <t>Heavy Gunner</t>
   </si>
   <si>
+    <t>Ghoul Auger Alpha</t>
+  </si>
+  <si>
+    <t>Quartakk Blueprint</t>
+  </si>
+  <si>
     <t>Grineer Manic</t>
   </si>
   <si>
@@ -161,12 +167,6 @@
     <t>0.2256</t>
   </si>
   <si>
-    <t>Ghoul Auger Alpha</t>
-  </si>
-  <si>
-    <t>Quartakk Blueprint</t>
-  </si>
-  <si>
     <t>Corrupted Warden</t>
   </si>
   <si>
@@ -230,6 +230,9 @@
     <t>0.015</t>
   </si>
   <si>
+    <t>Kuva Hyekka Master</t>
+  </si>
+  <si>
     <t>Zanuka Hunter</t>
   </si>
   <si>
@@ -237,9 +240,6 @@
   </si>
   <si>
     <t>Scimitar Avionics Blueprint</t>
-  </si>
-  <si>
-    <t>Kuva Hyekka Master</t>
   </si>
   <si>
     <t>Vem Tabook</t>
@@ -513,42 +513,42 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -737,7 +737,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>67</v>
@@ -746,7 +746,7 @@
         <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
         <v>68</v>
@@ -755,7 +755,7 @@
         <v>36</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
@@ -777,36 +777,36 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22">

</xml_diff>